<commit_message>
Committing changes for the new test cases written as of 03/05/2025
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs002430_Race-Asian.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs002430_Race-Asian.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/CCDI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\12-16-24\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16755EA-5DF2-4F4F-97CD-29A6CF2C9511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB95FEBF-EB5C-4A63-B331-FD942E941A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41180" yWindow="220" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,25 +75,6 @@
   </si>
   <si>
     <t>SELECT
-    COUNT(DISTINCT st.study_id) AS "Studies",
-    COUNT(DISTINCT p.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    COUNT(DISTINCT sf.id) AS "Files"
-FROM 
-    df_participant p
-JOIN 
-    df_study st ON p."study.id" = st.id
-LEFT JOIN 
-    df_sample smp ON smp."participant.id" = p.id
-LEFT JOIN 
-    df_sequencing_file sf ON sf."sample.id" = smp.id
-LEFT JOIN 
-    df_methylation_array_file maf ON maf."sample.id" = smp.sample_id
-WHERE 
-    st.study_id = 'phs002430' AND p.race = 'Asian';</t>
-  </si>
-  <si>
-    <t>SELECT
     p.participant_id AS "Participant ID",
     st.study_id AS "Study ID",
     COALESCE(p.sex_at_birth, '') AS "Sex",
@@ -253,6 +234,27 @@
 ORDER BY 
     sqf.file_name ASC
 LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT
+    COUNT(DISTINCT std.study_ID) AS "Studies",
+    COUNT(DISTINCT prt.participant_id) AS "Participants",
+    COUNT(DISTINCT smp.sample_id) AS "Samples",
+    (COUNT(DISTINCT seq.id) + COUNT(DISTINCT paf.id)) AS "Files"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN 
+    df_sequencing_file seq ON smp.id = seq."sample.id"
+LEFT JOIN 
+    df_pathology_file paf ON smp.id = paf."sample.id"
+WHERE 
+    std.study_ID = 'phs002430' 
+    AND prt.race = 'Asian' 
+    AND prt.sex_at_birth = 'Female';</t>
   </si>
 </sst>
 </file>
@@ -654,19 +656,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.83203125" customWidth="1"/>
-    <col min="4" max="4" width="70.1640625" customWidth="1"/>
-    <col min="5" max="5" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.140625" customWidth="1"/>
+    <col min="5" max="5" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -683,15 +685,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="404" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="378" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -700,47 +702,47 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ccdi testcases from ashwini1212 branch
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs002430_Race-Asian.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs002430_Race-Asian.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/CCDI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\12-16-24\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16755EA-5DF2-4F4F-97CD-29A6CF2C9511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB95FEBF-EB5C-4A63-B331-FD942E941A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41180" yWindow="220" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,25 +75,6 @@
   </si>
   <si>
     <t>SELECT
-    COUNT(DISTINCT st.study_id) AS "Studies",
-    COUNT(DISTINCT p.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    COUNT(DISTINCT sf.id) AS "Files"
-FROM 
-    df_participant p
-JOIN 
-    df_study st ON p."study.id" = st.id
-LEFT JOIN 
-    df_sample smp ON smp."participant.id" = p.id
-LEFT JOIN 
-    df_sequencing_file sf ON sf."sample.id" = smp.id
-LEFT JOIN 
-    df_methylation_array_file maf ON maf."sample.id" = smp.sample_id
-WHERE 
-    st.study_id = 'phs002430' AND p.race = 'Asian';</t>
-  </si>
-  <si>
-    <t>SELECT
     p.participant_id AS "Participant ID",
     st.study_id AS "Study ID",
     COALESCE(p.sex_at_birth, '') AS "Sex",
@@ -253,6 +234,27 @@
 ORDER BY 
     sqf.file_name ASC
 LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT
+    COUNT(DISTINCT std.study_ID) AS "Studies",
+    COUNT(DISTINCT prt.participant_id) AS "Participants",
+    COUNT(DISTINCT smp.sample_id) AS "Samples",
+    (COUNT(DISTINCT seq.id) + COUNT(DISTINCT paf.id)) AS "Files"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN 
+    df_sequencing_file seq ON smp.id = seq."sample.id"
+LEFT JOIN 
+    df_pathology_file paf ON smp.id = paf."sample.id"
+WHERE 
+    std.study_ID = 'phs002430' 
+    AND prt.race = 'Asian' 
+    AND prt.sex_at_birth = 'Female';</t>
   </si>
 </sst>
 </file>
@@ -654,19 +656,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.83203125" customWidth="1"/>
-    <col min="4" max="4" width="70.1640625" customWidth="1"/>
-    <col min="5" max="5" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.140625" customWidth="1"/>
+    <col min="5" max="5" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -683,15 +685,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="404" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="378" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -700,47 +702,47 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
   </sheetData>

</xml_diff>